<commit_message>
update assertion excel sheet
</commit_message>
<xml_diff>
--- a/packages/assertions/assertions.xlsx
+++ b/packages/assertions/assertions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="assertions" sheetId="1" r:id="rId1"/>
@@ -2481,7 +2481,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2507,6 +2507,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2883,23 +2886,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IN307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A307" sqref="A307:G307"/>
+    <sheetView tabSelected="1" topLeftCell="A296" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D318" sqref="D318"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="101.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="101.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="46.5546875" customWidth="1"/>
-    <col min="8" max="8" width="91.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="8" max="8" width="91.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:248" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="2" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -2941,7 +2944,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2957,7 +2960,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -2973,7 +2976,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2987,7 +2990,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
@@ -3249,7 +3252,7 @@
       <c r="IM6"/>
       <c r="IN6"/>
     </row>
-    <row r="7" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
@@ -3269,7 +3272,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -3531,7 +3534,7 @@
       <c r="IM8"/>
       <c r="IN8"/>
     </row>
-    <row r="9" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -3793,7 +3796,7 @@
       <c r="IM9"/>
       <c r="IN9"/>
     </row>
-    <row r="10" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -4055,7 +4058,7 @@
       <c r="IM10"/>
       <c r="IN10"/>
     </row>
-    <row r="11" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -4317,7 +4320,7 @@
       <c r="IM11"/>
       <c r="IN11"/>
     </row>
-    <row r="12" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -4579,7 +4582,7 @@
       <c r="IM12"/>
       <c r="IN12"/>
     </row>
-    <row r="13" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -4841,7 +4844,7 @@
       <c r="IM13"/>
       <c r="IN13"/>
     </row>
-    <row r="14" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -5103,7 +5106,7 @@
       <c r="IM14"/>
       <c r="IN14"/>
     </row>
-    <row r="15" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -5365,7 +5368,7 @@
       <c r="IM15"/>
       <c r="IN15"/>
     </row>
-    <row r="16" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
@@ -5383,7 +5386,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
@@ -5645,7 +5648,7 @@
       <c r="IM17"/>
       <c r="IN17"/>
     </row>
-    <row r="18" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:248" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
@@ -5667,7 +5670,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
@@ -5685,7 +5688,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -5703,7 +5706,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:248" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:248" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>49</v>
       </c>
@@ -5721,7 +5724,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -5983,7 +5986,7 @@
       <c r="IM22"/>
       <c r="IN22"/>
     </row>
-    <row r="23" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>55</v>
       </c>
@@ -6245,7 +6248,7 @@
       <c r="IM23"/>
       <c r="IN23"/>
     </row>
-    <row r="24" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>57</v>
       </c>
@@ -6507,7 +6510,7 @@
       <c r="IM24"/>
       <c r="IN24"/>
     </row>
-    <row r="25" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -6769,7 +6772,7 @@
       <c r="IM25"/>
       <c r="IN25"/>
     </row>
-    <row r="26" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
@@ -7029,7 +7032,7 @@
       <c r="IM26"/>
       <c r="IN26"/>
     </row>
-    <row r="27" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>62</v>
       </c>
@@ -7289,7 +7292,7 @@
       <c r="IM27"/>
       <c r="IN27"/>
     </row>
-    <row r="28" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:248" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>64</v>
       </c>
@@ -7549,7 +7552,7 @@
       <c r="IM28"/>
       <c r="IN28"/>
     </row>
-    <row r="29" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>66</v>
       </c>
@@ -7809,7 +7812,7 @@
       <c r="IM29"/>
       <c r="IN29"/>
     </row>
-    <row r="30" spans="1:248" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:248" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>68</v>
       </c>
@@ -8069,7 +8072,7 @@
       <c r="IM30"/>
       <c r="IN30"/>
     </row>
-    <row r="31" spans="1:248" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:248" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>70</v>
       </c>
@@ -8329,7 +8332,7 @@
       <c r="IM31"/>
       <c r="IN31"/>
     </row>
-    <row r="32" spans="1:248" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:248" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>74</v>
       </c>
@@ -8589,7 +8592,7 @@
       <c r="IM32"/>
       <c r="IN32"/>
     </row>
-    <row r="33" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>77</v>
       </c>
@@ -8849,7 +8852,7 @@
       <c r="IM33"/>
       <c r="IN33"/>
     </row>
-    <row r="34" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>79</v>
       </c>
@@ -9109,7 +9112,7 @@
       <c r="IM34"/>
       <c r="IN34"/>
     </row>
-    <row r="35" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>81</v>
       </c>
@@ -9369,7 +9372,7 @@
       <c r="IM35"/>
       <c r="IN35"/>
     </row>
-    <row r="36" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:248" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>83</v>
       </c>
@@ -9387,7 +9390,7 @@
       <c r="G36" s="9"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>98</v>
       </c>
@@ -9649,7 +9652,7 @@
       <c r="IM37"/>
       <c r="IN37"/>
     </row>
-    <row r="38" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>100</v>
       </c>
@@ -9911,7 +9914,7 @@
       <c r="IM38"/>
       <c r="IN38"/>
     </row>
-    <row r="39" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>102</v>
       </c>
@@ -10173,7 +10176,7 @@
       <c r="IM39"/>
       <c r="IN39"/>
     </row>
-    <row r="40" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>104</v>
       </c>
@@ -10435,7 +10438,7 @@
       <c r="IM40"/>
       <c r="IN40"/>
     </row>
-    <row r="41" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>106</v>
       </c>
@@ -10697,7 +10700,7 @@
       <c r="IM41"/>
       <c r="IN41"/>
     </row>
-    <row r="42" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>108</v>
       </c>
@@ -10957,7 +10960,7 @@
       <c r="IM42"/>
       <c r="IN42"/>
     </row>
-    <row r="43" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>110</v>
       </c>
@@ -11219,7 +11222,7 @@
       <c r="IM43"/>
       <c r="IN43"/>
     </row>
-    <row r="44" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>115</v>
       </c>
@@ -11481,7 +11484,7 @@
       <c r="IM44"/>
       <c r="IN44"/>
     </row>
-    <row r="45" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>118</v>
       </c>
@@ -11743,7 +11746,7 @@
       <c r="IM45"/>
       <c r="IN45"/>
     </row>
-    <row r="46" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>113</v>
       </c>
@@ -12005,7 +12008,7 @@
       <c r="IM46"/>
       <c r="IN46"/>
     </row>
-    <row r="47" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>123</v>
       </c>
@@ -12267,7 +12270,7 @@
       <c r="IM47"/>
       <c r="IN47"/>
     </row>
-    <row r="48" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>125</v>
       </c>
@@ -12529,7 +12532,7 @@
       <c r="IM48"/>
       <c r="IN48"/>
     </row>
-    <row r="49" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>121</v>
       </c>
@@ -12791,7 +12794,7 @@
       <c r="IM49"/>
       <c r="IN49"/>
     </row>
-    <row r="50" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>127</v>
       </c>
@@ -13053,7 +13056,7 @@
       <c r="IM50"/>
       <c r="IN50"/>
     </row>
-    <row r="51" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>129</v>
       </c>
@@ -13315,7 +13318,7 @@
       <c r="IM51"/>
       <c r="IN51"/>
     </row>
-    <row r="52" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>132</v>
       </c>
@@ -13577,7 +13580,7 @@
       <c r="IM52"/>
       <c r="IN52"/>
     </row>
-    <row r="53" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>134</v>
       </c>
@@ -13839,7 +13842,7 @@
       <c r="IM53"/>
       <c r="IN53"/>
     </row>
-    <row r="54" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>136</v>
       </c>
@@ -14101,7 +14104,7 @@
       <c r="IM54"/>
       <c r="IN54"/>
     </row>
-    <row r="55" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>138</v>
       </c>
@@ -14363,7 +14366,7 @@
       <c r="IM55"/>
       <c r="IN55"/>
     </row>
-    <row r="56" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>140</v>
       </c>
@@ -14625,7 +14628,7 @@
       <c r="IM56"/>
       <c r="IN56"/>
     </row>
-    <row r="57" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>142</v>
       </c>
@@ -14887,7 +14890,7 @@
       <c r="IM57"/>
       <c r="IN57"/>
     </row>
-    <row r="58" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>144</v>
       </c>
@@ -15149,7 +15152,7 @@
       <c r="IM58"/>
       <c r="IN58"/>
     </row>
-    <row r="59" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>86</v>
       </c>
@@ -15169,7 +15172,7 @@
       <c r="G59" s="9"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>88</v>
       </c>
@@ -15431,7 +15434,7 @@
       <c r="IM60"/>
       <c r="IN60"/>
     </row>
-    <row r="61" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>90</v>
       </c>
@@ -15693,7 +15696,7 @@
       <c r="IM61"/>
       <c r="IN61"/>
     </row>
-    <row r="62" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>92</v>
       </c>
@@ -15955,7 +15958,7 @@
       <c r="IM62"/>
       <c r="IN62"/>
     </row>
-    <row r="63" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>94</v>
       </c>
@@ -16217,7 +16220,7 @@
       <c r="IM63"/>
       <c r="IN63"/>
     </row>
-    <row r="64" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>96</v>
       </c>
@@ -16479,7 +16482,7 @@
       <c r="IM64"/>
       <c r="IN64"/>
     </row>
-    <row r="65" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>146</v>
       </c>
@@ -16739,7 +16742,7 @@
       <c r="IM65"/>
       <c r="IN65"/>
     </row>
-    <row r="66" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>148</v>
       </c>
@@ -16999,7 +17002,7 @@
       <c r="IM66"/>
       <c r="IN66"/>
     </row>
-    <row r="67" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>150</v>
       </c>
@@ -17019,7 +17022,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>154</v>
       </c>
@@ -17041,7 +17044,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>159</v>
       </c>
@@ -17061,7 +17064,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>161</v>
       </c>
@@ -17323,7 +17326,7 @@
       <c r="IM70"/>
       <c r="IN70"/>
     </row>
-    <row r="71" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>165</v>
       </c>
@@ -17343,7 +17346,7 @@
       <c r="G71" s="9"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>167</v>
       </c>
@@ -17601,7 +17604,7 @@
       <c r="IM72"/>
       <c r="IN72"/>
     </row>
-    <row r="73" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>169</v>
       </c>
@@ -17863,7 +17866,7 @@
       <c r="IM73"/>
       <c r="IN73"/>
     </row>
-    <row r="74" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>171</v>
       </c>
@@ -18125,7 +18128,7 @@
       <c r="IM74"/>
       <c r="IN74"/>
     </row>
-    <row r="75" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>173</v>
       </c>
@@ -18387,7 +18390,7 @@
       <c r="IM75"/>
       <c r="IN75"/>
     </row>
-    <row r="76" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>175</v>
       </c>
@@ -18649,7 +18652,7 @@
       <c r="IM76"/>
       <c r="IN76"/>
     </row>
-    <row r="77" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>177</v>
       </c>
@@ -18669,7 +18672,7 @@
       <c r="G77" s="9"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>179</v>
       </c>
@@ -18931,7 +18934,7 @@
       <c r="IM78"/>
       <c r="IN78"/>
     </row>
-    <row r="79" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>181</v>
       </c>
@@ -19193,7 +19196,7 @@
       <c r="IM79"/>
       <c r="IN79"/>
     </row>
-    <row r="80" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>183</v>
       </c>
@@ -19455,7 +19458,7 @@
       <c r="IM80"/>
       <c r="IN80"/>
     </row>
-    <row r="81" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>164</v>
       </c>
@@ -19473,7 +19476,7 @@
       <c r="G81" s="9"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>186</v>
       </c>
@@ -19735,7 +19738,7 @@
       <c r="IM82"/>
       <c r="IN82"/>
     </row>
-    <row r="83" spans="1:248" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:248" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>188</v>
       </c>
@@ -19995,7 +19998,7 @@
       <c r="IM83"/>
       <c r="IN83"/>
     </row>
-    <row r="84" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>194</v>
       </c>
@@ -20257,7 +20260,7 @@
       <c r="IM84"/>
       <c r="IN84"/>
     </row>
-    <row r="85" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>190</v>
       </c>
@@ -20519,7 +20522,7 @@
       <c r="IM85"/>
       <c r="IN85"/>
     </row>
-    <row r="86" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>193</v>
       </c>
@@ -20779,7 +20782,7 @@
       <c r="IM86"/>
       <c r="IN86"/>
     </row>
-    <row r="87" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>197</v>
       </c>
@@ -21039,7 +21042,7 @@
       <c r="IM87"/>
       <c r="IN87"/>
     </row>
-    <row r="88" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>199</v>
       </c>
@@ -21299,7 +21302,7 @@
       <c r="IM88"/>
       <c r="IN88"/>
     </row>
-    <row r="89" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>204</v>
       </c>
@@ -21561,7 +21564,7 @@
       <c r="IM89"/>
       <c r="IN89"/>
     </row>
-    <row r="90" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>207</v>
       </c>
@@ -21823,7 +21826,7 @@
       <c r="IM90"/>
       <c r="IN90"/>
     </row>
-    <row r="91" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>201</v>
       </c>
@@ -22085,7 +22088,7 @@
       <c r="IM91"/>
       <c r="IN91"/>
     </row>
-    <row r="92" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>210</v>
       </c>
@@ -22345,7 +22348,7 @@
       <c r="IM92"/>
       <c r="IN92"/>
     </row>
-    <row r="93" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>212</v>
       </c>
@@ -22605,7 +22608,7 @@
       <c r="IM93"/>
       <c r="IN93"/>
     </row>
-    <row r="94" spans="1:248" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:248" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>222</v>
       </c>
@@ -22863,7 +22866,7 @@
       <c r="IM94"/>
       <c r="IN94"/>
     </row>
-    <row r="95" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>214</v>
       </c>
@@ -22881,7 +22884,7 @@
       <c r="G95" s="9"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>218</v>
       </c>
@@ -23143,7 +23146,7 @@
       <c r="IM96"/>
       <c r="IN96"/>
     </row>
-    <row r="97" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>220</v>
       </c>
@@ -23405,7 +23408,7 @@
       <c r="IM97"/>
       <c r="IN97"/>
     </row>
-    <row r="98" spans="1:248" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:248" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>216</v>
       </c>
@@ -23663,7 +23666,7 @@
       <c r="IM98"/>
       <c r="IN98"/>
     </row>
-    <row r="99" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>225</v>
       </c>
@@ -23921,7 +23924,7 @@
       <c r="IM99"/>
       <c r="IN99"/>
     </row>
-    <row r="100" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>227</v>
       </c>
@@ -24179,7 +24182,7 @@
       <c r="IM100"/>
       <c r="IN100"/>
     </row>
-    <row r="101" spans="1:248" ht="72" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:248" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>229</v>
       </c>
@@ -24197,7 +24200,7 @@
       <c r="G101" s="9"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>232</v>
       </c>
@@ -24459,7 +24462,7 @@
       <c r="IM102"/>
       <c r="IN102"/>
     </row>
-    <row r="103" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>234</v>
       </c>
@@ -24721,7 +24724,7 @@
       <c r="IM103"/>
       <c r="IN103"/>
     </row>
-    <row r="104" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>236</v>
       </c>
@@ -24983,7 +24986,7 @@
       <c r="IM104"/>
       <c r="IN104"/>
     </row>
-    <row r="105" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>238</v>
       </c>
@@ -25245,7 +25248,7 @@
       <c r="IM105"/>
       <c r="IN105"/>
     </row>
-    <row r="106" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>240</v>
       </c>
@@ -25507,7 +25510,7 @@
       <c r="IM106"/>
       <c r="IN106"/>
     </row>
-    <row r="107" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>242</v>
       </c>
@@ -25769,7 +25772,7 @@
       <c r="IM107"/>
       <c r="IN107"/>
     </row>
-    <row r="108" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>244</v>
       </c>
@@ -26031,7 +26034,7 @@
       <c r="IM108"/>
       <c r="IN108"/>
     </row>
-    <row r="109" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>246</v>
       </c>
@@ -26293,7 +26296,7 @@
       <c r="IM109"/>
       <c r="IN109"/>
     </row>
-    <row r="110" spans="1:248" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:248" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>248</v>
       </c>
@@ -26555,7 +26558,7 @@
       <c r="IM110"/>
       <c r="IN110"/>
     </row>
-    <row r="111" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>250</v>
       </c>
@@ -26815,7 +26818,7 @@
       <c r="IM111"/>
       <c r="IN111"/>
     </row>
-    <row r="112" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>253</v>
       </c>
@@ -26833,7 +26836,7 @@
       <c r="G112" s="9"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>255</v>
       </c>
@@ -27095,7 +27098,7 @@
       <c r="IM113"/>
       <c r="IN113"/>
     </row>
-    <row r="114" spans="1:248" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:248" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
         <v>257</v>
       </c>
@@ -27355,7 +27358,7 @@
       <c r="IM114"/>
       <c r="IN114"/>
     </row>
-    <row r="115" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>259</v>
       </c>
@@ -27617,7 +27620,7 @@
       <c r="IM115"/>
       <c r="IN115"/>
     </row>
-    <row r="116" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:248" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>261</v>
       </c>
@@ -27637,7 +27640,7 @@
       <c r="G116" s="9"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>263</v>
       </c>
@@ -27899,7 +27902,7 @@
       <c r="IM117"/>
       <c r="IN117"/>
     </row>
-    <row r="118" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>265</v>
       </c>
@@ -28161,7 +28164,7 @@
       <c r="IM118"/>
       <c r="IN118"/>
     </row>
-    <row r="119" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>267</v>
       </c>
@@ -28423,7 +28426,7 @@
       <c r="IM119"/>
       <c r="IN119"/>
     </row>
-    <row r="120" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>269</v>
       </c>
@@ -28443,7 +28446,7 @@
       <c r="G120" s="9"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>272</v>
       </c>
@@ -28705,7 +28708,7 @@
       <c r="IM121"/>
       <c r="IN121"/>
     </row>
-    <row r="122" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>274</v>
       </c>
@@ -28967,7 +28970,7 @@
       <c r="IM122"/>
       <c r="IN122"/>
     </row>
-    <row r="123" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>277</v>
       </c>
@@ -29223,7 +29226,7 @@
       <c r="IM123"/>
       <c r="IN123"/>
     </row>
-    <row r="124" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>279</v>
       </c>
@@ -29479,18 +29482,21 @@
       <c r="IM124"/>
       <c r="IN124"/>
     </row>
-    <row r="125" spans="1:248" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+    <row r="125" spans="1:248" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="7"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:248" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>283</v>
       </c>
@@ -29506,7 +29512,7 @@
       <c r="G126" s="6"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>285</v>
       </c>
@@ -29517,7 +29523,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>287</v>
       </c>
@@ -29779,7 +29785,7 @@
       <c r="IM128"/>
       <c r="IN128"/>
     </row>
-    <row r="129" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>289</v>
       </c>
@@ -29793,7 +29799,7 @@
       <c r="G129" s="6"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:248" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>291</v>
       </c>
@@ -29809,7 +29815,7 @@
       <c r="G130" s="7"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:248" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>293</v>
       </c>
@@ -29825,7 +29831,7 @@
       <c r="G131" s="7"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>295</v>
       </c>
@@ -30087,7 +30093,7 @@
       <c r="IM132"/>
       <c r="IN132"/>
     </row>
-    <row r="133" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:248" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>298</v>
       </c>
@@ -30103,20 +30109,23 @@
       <c r="G133" s="7"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:248" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:248" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="B134" s="11"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
+      <c r="G134" s="11"/>
       <c r="H134" s="1" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="135" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:248" s="3" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>302</v>
       </c>
@@ -30378,7 +30387,7 @@
       <c r="IM135"/>
       <c r="IN135"/>
     </row>
-    <row r="136" spans="1:248" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:248" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>304</v>
       </c>
@@ -30638,7 +30647,7 @@
       <c r="IM136"/>
       <c r="IN136"/>
     </row>
-    <row r="137" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:248" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>307</v>
       </c>
@@ -30900,20 +30909,23 @@
       <c r="IM137"/>
       <c r="IN137"/>
     </row>
-    <row r="138" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:248" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="B138" s="10"/>
+      <c r="C138" s="10"/>
+      <c r="D138" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="F138" s="1"/>
-      <c r="G138" s="1"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10"/>
+      <c r="G138" s="10"/>
       <c r="H138" s="1" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="139" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>311</v>
       </c>
@@ -31173,7 +31185,7 @@
       <c r="IM139"/>
       <c r="IN139"/>
     </row>
-    <row r="140" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>313</v>
       </c>
@@ -31191,7 +31203,7 @@
       <c r="G140" s="9"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>315</v>
       </c>
@@ -31453,7 +31465,7 @@
       <c r="IM141"/>
       <c r="IN141"/>
     </row>
-    <row r="142" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>317</v>
       </c>
@@ -31715,7 +31727,7 @@
       <c r="IM142"/>
       <c r="IN142"/>
     </row>
-    <row r="143" spans="1:248" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:248" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>319</v>
       </c>
@@ -31973,7 +31985,7 @@
       <c r="IM143"/>
       <c r="IN143"/>
     </row>
-    <row r="144" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>321</v>
       </c>
@@ -32233,7 +32245,7 @@
       <c r="IM144"/>
       <c r="IN144"/>
     </row>
-    <row r="145" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>324</v>
       </c>
@@ -32493,7 +32505,7 @@
       <c r="IM145"/>
       <c r="IN145"/>
     </row>
-    <row r="146" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>326</v>
       </c>
@@ -32753,7 +32765,7 @@
       <c r="IM146"/>
       <c r="IN146"/>
     </row>
-    <row r="147" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>330</v>
       </c>
@@ -33015,7 +33027,7 @@
       <c r="IM147"/>
       <c r="IN147"/>
     </row>
-    <row r="148" spans="1:248" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:248" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>334</v>
       </c>
@@ -33031,7 +33043,7 @@
       <c r="G148" s="7"/>
       <c r="H148" s="1"/>
     </row>
-    <row r="149" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>336</v>
       </c>
@@ -33293,7 +33305,7 @@
       <c r="IM149"/>
       <c r="IN149"/>
     </row>
-    <row r="150" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>339</v>
       </c>
@@ -33309,7 +33321,7 @@
       <c r="G150" s="7"/>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>341</v>
       </c>
@@ -33571,7 +33583,7 @@
       <c r="IM151"/>
       <c r="IN151"/>
     </row>
-    <row r="152" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>344</v>
       </c>
@@ -33833,7 +33845,7 @@
       <c r="IM152"/>
       <c r="IN152"/>
     </row>
-    <row r="153" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>346</v>
       </c>
@@ -34095,7 +34107,7 @@
       <c r="IM153"/>
       <c r="IN153"/>
     </row>
-    <row r="154" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>348</v>
       </c>
@@ -34357,7 +34369,7 @@
       <c r="IM154"/>
       <c r="IN154"/>
     </row>
-    <row r="155" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>350</v>
       </c>
@@ -34619,7 +34631,7 @@
       <c r="IM155"/>
       <c r="IN155"/>
     </row>
-    <row r="156" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>351</v>
       </c>
@@ -34881,7 +34893,7 @@
       <c r="IM156"/>
       <c r="IN156"/>
     </row>
-    <row r="157" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>352</v>
       </c>
@@ -35143,7 +35155,7 @@
       <c r="IM157"/>
       <c r="IN157"/>
     </row>
-    <row r="158" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>354</v>
       </c>
@@ -35405,7 +35417,7 @@
       <c r="IM158"/>
       <c r="IN158"/>
     </row>
-    <row r="159" spans="1:248" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:248" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>356</v>
       </c>
@@ -35667,7 +35679,7 @@
       <c r="IM159"/>
       <c r="IN159"/>
     </row>
-    <row r="160" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>358</v>
       </c>
@@ -35929,7 +35941,7 @@
       <c r="IM160"/>
       <c r="IN160"/>
     </row>
-    <row r="161" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>360</v>
       </c>
@@ -36191,7 +36203,7 @@
       <c r="IM161"/>
       <c r="IN161"/>
     </row>
-    <row r="162" spans="1:248" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:248" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>362</v>
       </c>
@@ -36453,7 +36465,7 @@
       <c r="IM162"/>
       <c r="IN162"/>
     </row>
-    <row r="163" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>364</v>
       </c>
@@ -36467,7 +36479,7 @@
       <c r="G163" s="7"/>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>366</v>
       </c>
@@ -36481,7 +36493,7 @@
       <c r="G164" s="7"/>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>368</v>
       </c>
@@ -36495,7 +36507,7 @@
       <c r="G165" s="7"/>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>370</v>
       </c>
@@ -36515,7 +36527,7 @@
       <c r="G166" s="7"/>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>373</v>
       </c>
@@ -36777,7 +36789,7 @@
       <c r="IM167"/>
       <c r="IN167"/>
     </row>
-    <row r="168" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>374</v>
       </c>
@@ -37039,7 +37051,7 @@
       <c r="IM168"/>
       <c r="IN168"/>
     </row>
-    <row r="169" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>376</v>
       </c>
@@ -37301,7 +37313,7 @@
       <c r="IM169"/>
       <c r="IN169"/>
     </row>
-    <row r="170" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>378</v>
       </c>
@@ -37315,7 +37327,7 @@
       <c r="G170" s="7"/>
       <c r="H170" s="1"/>
     </row>
-    <row r="171" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>380</v>
       </c>
@@ -37577,7 +37589,7 @@
       <c r="IM171"/>
       <c r="IN171"/>
     </row>
-    <row r="172" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>382</v>
       </c>
@@ -37839,7 +37851,7 @@
       <c r="IM172"/>
       <c r="IN172"/>
     </row>
-    <row r="173" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
         <v>385</v>
       </c>
@@ -38101,7 +38113,7 @@
       <c r="IM173"/>
       <c r="IN173"/>
     </row>
-    <row r="174" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>383</v>
       </c>
@@ -38363,7 +38375,7 @@
       <c r="IM174"/>
       <c r="IN174"/>
     </row>
-    <row r="175" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
         <v>387</v>
       </c>
@@ -38625,7 +38637,7 @@
       <c r="IM175"/>
       <c r="IN175"/>
     </row>
-    <row r="176" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
         <v>388</v>
       </c>
@@ -38887,7 +38899,7 @@
       <c r="IM176"/>
       <c r="IN176"/>
     </row>
-    <row r="177" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>389</v>
       </c>
@@ -39149,7 +39161,7 @@
       <c r="IM177"/>
       <c r="IN177"/>
     </row>
-    <row r="178" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>384</v>
       </c>
@@ -39411,7 +39423,7 @@
       <c r="IM178"/>
       <c r="IN178"/>
     </row>
-    <row r="179" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>390</v>
       </c>
@@ -39673,7 +39685,7 @@
       <c r="IM179"/>
       <c r="IN179"/>
     </row>
-    <row r="180" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>392</v>
       </c>
@@ -39935,7 +39947,7 @@
       <c r="IM180"/>
       <c r="IN180"/>
     </row>
-    <row r="181" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>394</v>
       </c>
@@ -39949,7 +39961,7 @@
       <c r="G181" s="7"/>
       <c r="H181" s="1"/>
     </row>
-    <row r="182" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>396</v>
       </c>
@@ -39963,7 +39975,7 @@
       <c r="G182" s="7"/>
       <c r="H182" s="1"/>
     </row>
-    <row r="183" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>398</v>
       </c>
@@ -39977,7 +39989,7 @@
       <c r="G183" s="7"/>
       <c r="H183" s="1"/>
     </row>
-    <row r="184" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>400</v>
       </c>
@@ -39991,7 +40003,7 @@
       <c r="G184" s="7"/>
       <c r="H184" s="1"/>
     </row>
-    <row r="185" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
         <v>402</v>
       </c>
@@ -40253,7 +40265,7 @@
       <c r="IM185"/>
       <c r="IN185"/>
     </row>
-    <row r="186" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
         <v>404</v>
       </c>
@@ -40515,7 +40527,7 @@
       <c r="IM186"/>
       <c r="IN186"/>
     </row>
-    <row r="187" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
         <v>406</v>
       </c>
@@ -40777,7 +40789,7 @@
       <c r="IM187"/>
       <c r="IN187"/>
     </row>
-    <row r="188" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>408</v>
       </c>
@@ -41039,7 +41051,7 @@
       <c r="IM188"/>
       <c r="IN188"/>
     </row>
-    <row r="189" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>410</v>
       </c>
@@ -41301,7 +41313,7 @@
       <c r="IM189"/>
       <c r="IN189"/>
     </row>
-    <row r="190" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>412</v>
       </c>
@@ -41563,7 +41575,7 @@
       <c r="IM190"/>
       <c r="IN190"/>
     </row>
-    <row r="191" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>414</v>
       </c>
@@ -41825,7 +41837,7 @@
       <c r="IM191"/>
       <c r="IN191"/>
     </row>
-    <row r="192" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>417</v>
       </c>
@@ -42087,7 +42099,7 @@
       <c r="IM192"/>
       <c r="IN192"/>
     </row>
-    <row r="193" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>419</v>
       </c>
@@ -42349,7 +42361,7 @@
       <c r="IM193"/>
       <c r="IN193"/>
     </row>
-    <row r="194" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>415</v>
       </c>
@@ -42611,7 +42623,7 @@
       <c r="IM194"/>
       <c r="IN194"/>
     </row>
-    <row r="195" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
         <v>422</v>
       </c>
@@ -42873,7 +42885,7 @@
       <c r="IM195"/>
       <c r="IN195"/>
     </row>
-    <row r="196" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>425</v>
       </c>
@@ -43135,7 +43147,7 @@
       <c r="IM196"/>
       <c r="IN196"/>
     </row>
-    <row r="197" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>427</v>
       </c>
@@ -43397,7 +43409,7 @@
       <c r="IM197"/>
       <c r="IN197"/>
     </row>
-    <row r="198" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>428</v>
       </c>
@@ -43659,7 +43671,7 @@
       <c r="IM198"/>
       <c r="IN198"/>
     </row>
-    <row r="199" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>430</v>
       </c>
@@ -43921,7 +43933,7 @@
       <c r="IM199"/>
       <c r="IN199"/>
     </row>
-    <row r="200" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>432</v>
       </c>
@@ -44183,7 +44195,7 @@
       <c r="IM200"/>
       <c r="IN200"/>
     </row>
-    <row r="201" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>435</v>
       </c>
@@ -44445,7 +44457,7 @@
       <c r="IM201"/>
       <c r="IN201"/>
     </row>
-    <row r="202" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>437</v>
       </c>
@@ -44707,7 +44719,7 @@
       <c r="IM202"/>
       <c r="IN202"/>
     </row>
-    <row r="203" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>443</v>
       </c>
@@ -44969,7 +44981,7 @@
       <c r="IM203"/>
       <c r="IN203"/>
     </row>
-    <row r="204" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>445</v>
       </c>
@@ -45231,7 +45243,7 @@
       <c r="IM204"/>
       <c r="IN204"/>
     </row>
-    <row r="205" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
         <v>439</v>
       </c>
@@ -45493,7 +45505,7 @@
       <c r="IM205"/>
       <c r="IN205"/>
     </row>
-    <row r="206" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>441</v>
       </c>
@@ -45507,7 +45519,7 @@
       <c r="G206" s="7"/>
       <c r="H206" s="1"/>
     </row>
-    <row r="207" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
         <v>451</v>
       </c>
@@ -45769,7 +45781,7 @@
       <c r="IM207"/>
       <c r="IN207"/>
     </row>
-    <row r="208" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>453</v>
       </c>
@@ -46031,7 +46043,7 @@
       <c r="IM208"/>
       <c r="IN208"/>
     </row>
-    <row r="209" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
         <v>447</v>
       </c>
@@ -46293,7 +46305,7 @@
       <c r="IM209"/>
       <c r="IN209"/>
     </row>
-    <row r="210" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
         <v>449</v>
       </c>
@@ -46307,7 +46319,7 @@
       <c r="G210" s="7"/>
       <c r="H210" s="1"/>
     </row>
-    <row r="211" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:248" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
         <v>455</v>
       </c>
@@ -46321,7 +46333,7 @@
       <c r="G211" s="7"/>
       <c r="H211" s="1"/>
     </row>
-    <row r="212" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>457</v>
       </c>
@@ -46581,7 +46593,7 @@
       <c r="IM212"/>
       <c r="IN212"/>
     </row>
-    <row r="213" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>459</v>
       </c>
@@ -46595,7 +46607,7 @@
       <c r="G213" s="7"/>
       <c r="H213" s="1"/>
     </row>
-    <row r="214" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>461</v>
       </c>
@@ -46609,7 +46621,7 @@
       <c r="G214" s="7"/>
       <c r="H214" s="1"/>
     </row>
-    <row r="215" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>463</v>
       </c>
@@ -46871,7 +46883,7 @@
       <c r="IM215"/>
       <c r="IN215"/>
     </row>
-    <row r="216" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
         <v>465</v>
       </c>
@@ -47133,7 +47145,7 @@
       <c r="IM216"/>
       <c r="IN216"/>
     </row>
-    <row r="217" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
         <v>466</v>
       </c>
@@ -47395,7 +47407,7 @@
       <c r="IM217"/>
       <c r="IN217"/>
     </row>
-    <row r="218" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
         <v>467</v>
       </c>
@@ -47657,7 +47669,7 @@
       <c r="IM218"/>
       <c r="IN218"/>
     </row>
-    <row r="219" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
         <v>468</v>
       </c>
@@ -47919,7 +47931,7 @@
       <c r="IM219"/>
       <c r="IN219"/>
     </row>
-    <row r="220" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
         <v>470</v>
       </c>
@@ -47933,7 +47945,7 @@
       <c r="G220" s="7"/>
       <c r="H220" s="1"/>
     </row>
-    <row r="221" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
         <v>472</v>
       </c>
@@ -48195,7 +48207,7 @@
       <c r="IM221"/>
       <c r="IN221"/>
     </row>
-    <row r="222" spans="1:248" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:248" ht="135" x14ac:dyDescent="0.25">
       <c r="A222" s="9" t="s">
         <v>474</v>
       </c>
@@ -48215,7 +48227,7 @@
       <c r="G222" s="9"/>
       <c r="H222" s="1"/>
     </row>
-    <row r="223" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
         <v>476</v>
       </c>
@@ -48471,7 +48483,7 @@
       <c r="IM223"/>
       <c r="IN223"/>
     </row>
-    <row r="224" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
         <v>478</v>
       </c>
@@ -48727,7 +48739,7 @@
       <c r="IM224"/>
       <c r="IN224"/>
     </row>
-    <row r="225" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
         <v>480</v>
       </c>
@@ -48983,7 +48995,7 @@
       <c r="IM225"/>
       <c r="IN225"/>
     </row>
-    <row r="226" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>482</v>
       </c>
@@ -49239,7 +49251,7 @@
       <c r="IM226"/>
       <c r="IN226"/>
     </row>
-    <row r="227" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
         <v>484</v>
       </c>
@@ -49495,7 +49507,7 @@
       <c r="IM227"/>
       <c r="IN227"/>
     </row>
-    <row r="228" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
         <v>486</v>
       </c>
@@ -49751,7 +49763,7 @@
       <c r="IM228"/>
       <c r="IN228"/>
     </row>
-    <row r="229" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
         <v>488</v>
       </c>
@@ -50007,7 +50019,7 @@
       <c r="IM229"/>
       <c r="IN229"/>
     </row>
-    <row r="230" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
         <v>490</v>
       </c>
@@ -50263,7 +50275,7 @@
       <c r="IM230"/>
       <c r="IN230"/>
     </row>
-    <row r="231" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
         <v>492</v>
       </c>
@@ -50519,7 +50531,7 @@
       <c r="IM231"/>
       <c r="IN231"/>
     </row>
-    <row r="232" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
         <v>494</v>
       </c>
@@ -50775,7 +50787,7 @@
       <c r="IM232"/>
       <c r="IN232"/>
     </row>
-    <row r="233" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
         <v>496</v>
       </c>
@@ -51031,7 +51043,7 @@
       <c r="IM233"/>
       <c r="IN233"/>
     </row>
-    <row r="234" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
         <v>498</v>
       </c>
@@ -51293,7 +51305,7 @@
       <c r="IM234"/>
       <c r="IN234"/>
     </row>
-    <row r="235" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
         <v>500</v>
       </c>
@@ -51307,7 +51319,7 @@
       <c r="G235" s="7"/>
       <c r="H235" s="1"/>
     </row>
-    <row r="236" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
         <v>502</v>
       </c>
@@ -51321,7 +51333,7 @@
       <c r="G236" s="7"/>
       <c r="H236" s="1"/>
     </row>
-    <row r="237" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
         <v>504</v>
       </c>
@@ -51583,7 +51595,7 @@
       <c r="IM237"/>
       <c r="IN237"/>
     </row>
-    <row r="238" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
         <v>506</v>
       </c>
@@ -51845,7 +51857,7 @@
       <c r="IM238"/>
       <c r="IN238"/>
     </row>
-    <row r="239" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
         <v>508</v>
       </c>
@@ -52107,7 +52119,7 @@
       <c r="IM239"/>
       <c r="IN239"/>
     </row>
-    <row r="240" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
         <v>510</v>
       </c>
@@ -52369,7 +52381,7 @@
       <c r="IM240"/>
       <c r="IN240"/>
     </row>
-    <row r="241" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
         <v>512</v>
       </c>
@@ -52631,7 +52643,7 @@
       <c r="IM241"/>
       <c r="IN241"/>
     </row>
-    <row r="242" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
         <v>514</v>
       </c>
@@ -52893,7 +52905,7 @@
       <c r="IM242"/>
       <c r="IN242"/>
     </row>
-    <row r="243" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
         <v>516</v>
       </c>
@@ -53155,7 +53167,7 @@
       <c r="IM243"/>
       <c r="IN243"/>
     </row>
-    <row r="244" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
         <v>518</v>
       </c>
@@ -53417,7 +53429,7 @@
       <c r="IM244"/>
       <c r="IN244"/>
     </row>
-    <row r="245" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
         <v>520</v>
       </c>
@@ -53679,7 +53691,7 @@
       <c r="IM245"/>
       <c r="IN245"/>
     </row>
-    <row r="246" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
         <v>522</v>
       </c>
@@ -53941,7 +53953,7 @@
       <c r="IM246"/>
       <c r="IN246"/>
     </row>
-    <row r="247" spans="1:248" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
         <v>524</v>
       </c>
@@ -53955,7 +53967,7 @@
       <c r="G247" s="7"/>
       <c r="H247" s="1"/>
     </row>
-    <row r="248" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="7" t="s">
         <v>526</v>
       </c>
@@ -53969,7 +53981,7 @@
       <c r="G248" s="7"/>
       <c r="H248" s="1"/>
     </row>
-    <row r="249" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
         <v>528</v>
       </c>
@@ -54231,7 +54243,7 @@
       <c r="IM249"/>
       <c r="IN249"/>
     </row>
-    <row r="250" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="7" t="s">
         <v>530</v>
       </c>
@@ -54493,7 +54505,7 @@
       <c r="IM250"/>
       <c r="IN250"/>
     </row>
-    <row r="251" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="7" t="s">
         <v>532</v>
       </c>
@@ -54755,7 +54767,7 @@
       <c r="IM251"/>
       <c r="IN251"/>
     </row>
-    <row r="252" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="7" t="s">
         <v>534</v>
       </c>
@@ -55017,7 +55029,7 @@
       <c r="IM252"/>
       <c r="IN252"/>
     </row>
-    <row r="253" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" s="7" t="s">
         <v>536</v>
       </c>
@@ -55279,7 +55291,7 @@
       <c r="IM253"/>
       <c r="IN253"/>
     </row>
-    <row r="254" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="7" t="s">
         <v>538</v>
       </c>
@@ -55541,7 +55553,7 @@
       <c r="IM254"/>
       <c r="IN254"/>
     </row>
-    <row r="255" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A255" s="7" t="s">
         <v>541</v>
       </c>
@@ -55803,7 +55815,7 @@
       <c r="IM255"/>
       <c r="IN255"/>
     </row>
-    <row r="256" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="7" t="s">
         <v>543</v>
       </c>
@@ -56065,7 +56077,7 @@
       <c r="IM256"/>
       <c r="IN256"/>
     </row>
-    <row r="257" spans="1:248" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:248" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A257" s="7" t="s">
         <v>545</v>
       </c>
@@ -56327,7 +56339,7 @@
       <c r="IM257"/>
       <c r="IN257"/>
     </row>
-    <row r="258" spans="1:248" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:248" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A258" s="7" t="s">
         <v>547</v>
       </c>
@@ -56589,7 +56601,7 @@
       <c r="IM258"/>
       <c r="IN258"/>
     </row>
-    <row r="259" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="7" t="s">
         <v>548</v>
       </c>
@@ -56851,7 +56863,7 @@
       <c r="IM259"/>
       <c r="IN259"/>
     </row>
-    <row r="260" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="7" t="s">
         <v>550</v>
       </c>
@@ -57113,7 +57125,7 @@
       <c r="IM260"/>
       <c r="IN260"/>
     </row>
-    <row r="261" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
         <v>552</v>
       </c>
@@ -57127,7 +57139,7 @@
       <c r="G261" s="7"/>
       <c r="H261" s="1"/>
     </row>
-    <row r="262" spans="1:248" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:248" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A262" s="7" t="s">
         <v>554</v>
       </c>
@@ -57389,7 +57401,7 @@
       <c r="IM262"/>
       <c r="IN262"/>
     </row>
-    <row r="263" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
         <v>556</v>
       </c>
@@ -57651,7 +57663,7 @@
       <c r="IM263"/>
       <c r="IN263"/>
     </row>
-    <row r="264" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
         <v>558</v>
       </c>
@@ -57665,7 +57677,7 @@
       <c r="G264" s="7"/>
       <c r="H264" s="1"/>
     </row>
-    <row r="265" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="7" t="s">
         <v>560</v>
       </c>
@@ -57927,7 +57939,7 @@
       <c r="IM265"/>
       <c r="IN265"/>
     </row>
-    <row r="266" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>328</v>
       </c>
@@ -57938,7 +57950,7 @@
       <c r="G266" s="1"/>
       <c r="H266" s="1"/>
     </row>
-    <row r="267" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="7" t="s">
         <v>562</v>
       </c>
@@ -58200,7 +58212,7 @@
       <c r="IM267"/>
       <c r="IN267"/>
     </row>
-    <row r="268" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="7" t="s">
         <v>564</v>
       </c>
@@ -58462,7 +58474,7 @@
       <c r="IM268"/>
       <c r="IN268"/>
     </row>
-    <row r="269" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="7" t="s">
         <v>567</v>
       </c>
@@ -58724,7 +58736,7 @@
       <c r="IM269"/>
       <c r="IN269"/>
     </row>
-    <row r="270" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="7" t="s">
         <v>569</v>
       </c>
@@ -58986,7 +58998,7 @@
       <c r="IM270"/>
       <c r="IN270"/>
     </row>
-    <row r="271" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="7" t="s">
         <v>570</v>
       </c>
@@ -59248,7 +59260,7 @@
       <c r="IM271"/>
       <c r="IN271"/>
     </row>
-    <row r="272" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="7" t="s">
         <v>565</v>
       </c>
@@ -59510,7 +59522,7 @@
       <c r="IM272"/>
       <c r="IN272"/>
     </row>
-    <row r="273" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
         <v>571</v>
       </c>
@@ -59772,7 +59784,7 @@
       <c r="IM273"/>
       <c r="IN273"/>
     </row>
-    <row r="274" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:248" ht="45" x14ac:dyDescent="0.25">
       <c r="A274" s="9" t="s">
         <v>573</v>
       </c>
@@ -59792,7 +59804,7 @@
       <c r="G274" s="9"/>
       <c r="H274" s="1"/>
     </row>
-    <row r="275" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="7" t="s">
         <v>575</v>
       </c>
@@ -60048,7 +60060,7 @@
       <c r="IM275"/>
       <c r="IN275"/>
     </row>
-    <row r="276" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="7" t="s">
         <v>577</v>
       </c>
@@ -60304,7 +60316,7 @@
       <c r="IM276"/>
       <c r="IN276"/>
     </row>
-    <row r="277" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
         <v>579</v>
       </c>
@@ -60560,7 +60572,7 @@
       <c r="IM277"/>
       <c r="IN277"/>
     </row>
-    <row r="278" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" s="7" t="s">
         <v>581</v>
       </c>
@@ -60816,7 +60828,7 @@
       <c r="IM278"/>
       <c r="IN278"/>
     </row>
-    <row r="279" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="7" t="s">
         <v>583</v>
       </c>
@@ -61072,7 +61084,7 @@
       <c r="IM279"/>
       <c r="IN279"/>
     </row>
-    <row r="280" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A280" s="7" t="s">
         <v>585</v>
       </c>
@@ -61328,7 +61340,7 @@
       <c r="IM280"/>
       <c r="IN280"/>
     </row>
-    <row r="281" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="7" t="s">
         <v>587</v>
       </c>
@@ -61584,7 +61596,7 @@
       <c r="IM281"/>
       <c r="IN281"/>
     </row>
-    <row r="282" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
         <v>589</v>
       </c>
@@ -61846,7 +61858,7 @@
       <c r="IM282"/>
       <c r="IN282"/>
     </row>
-    <row r="283" spans="1:248" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A283" s="7" t="s">
         <v>591</v>
       </c>
@@ -62108,7 +62120,7 @@
       <c r="IM283"/>
       <c r="IN283"/>
     </row>
-    <row r="284" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:248" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A284" s="7" t="s">
         <v>593</v>
       </c>
@@ -62370,7 +62382,7 @@
       <c r="IM284"/>
       <c r="IN284"/>
     </row>
-    <row r="285" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:248" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="7" t="s">
         <v>595</v>
       </c>
@@ -62632,7 +62644,7 @@
       <c r="IM285"/>
       <c r="IN285"/>
     </row>
-    <row r="286" spans="1:248" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:248" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="7" t="s">
         <v>597</v>
       </c>
@@ -62894,7 +62906,7 @@
       <c r="IM286"/>
       <c r="IN286"/>
     </row>
-    <row r="287" spans="1:248" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="7" t="s">
         <v>599</v>
       </c>
@@ -62908,7 +62920,7 @@
       <c r="G287" s="7"/>
       <c r="H287" s="1"/>
     </row>
-    <row r="288" spans="1:248" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:248" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="7" t="s">
         <v>601</v>
       </c>
@@ -62922,7 +62934,7 @@
       <c r="G288" s="7"/>
       <c r="H288" s="1"/>
     </row>
-    <row r="289" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="7" t="s">
         <v>603</v>
       </c>
@@ -62936,7 +62948,7 @@
       <c r="G289" s="7"/>
       <c r="H289" s="1"/>
     </row>
-    <row r="290" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="7" t="s">
         <v>605</v>
       </c>
@@ -62950,7 +62962,7 @@
       <c r="G290" s="7"/>
       <c r="H290" s="1"/>
     </row>
-    <row r="291" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" s="7" t="s">
         <v>607</v>
       </c>
@@ -62964,7 +62976,7 @@
       <c r="G291" s="7"/>
       <c r="H291" s="1"/>
     </row>
-    <row r="292" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A292" s="10" t="s">
         <v>609</v>
       </c>
@@ -62978,7 +62990,7 @@
       <c r="G292" s="10"/>
       <c r="H292" s="1"/>
     </row>
-    <row r="293" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="10" t="s">
         <v>611</v>
       </c>
@@ -62992,7 +63004,7 @@
       <c r="G293" s="10"/>
       <c r="H293" s="1"/>
     </row>
-    <row r="294" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A294" s="7" t="s">
         <v>613</v>
       </c>
@@ -63006,42 +63018,51 @@
       <c r="G294" s="7"/>
       <c r="H294" s="1"/>
     </row>
-    <row r="295" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A295" s="1" t="s">
+    <row r="295" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A295" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="D295" s="1" t="s">
+      <c r="B295" s="7"/>
+      <c r="C295" s="7"/>
+      <c r="D295" s="7" t="s">
         <v>616</v>
       </c>
-      <c r="F295" s="1"/>
-      <c r="G295" s="1" t="s">
+      <c r="E295" s="7"/>
+      <c r="F295" s="7"/>
+      <c r="G295" s="7" t="s">
         <v>650</v>
       </c>
       <c r="H295" s="1"/>
     </row>
-    <row r="296" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A296" s="1" t="s">
+    <row r="296" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A296" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="D296" s="1" t="s">
+      <c r="B296" s="7"/>
+      <c r="C296" s="7"/>
+      <c r="D296" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="F296" s="1"/>
-      <c r="G296" s="1"/>
+      <c r="E296" s="7"/>
+      <c r="F296" s="7"/>
+      <c r="G296" s="7"/>
       <c r="H296" s="1"/>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A297" s="1" t="s">
+    <row r="297" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A297" s="10" t="s">
         <v>619</v>
       </c>
-      <c r="D297" s="1" t="s">
+      <c r="B297" s="10"/>
+      <c r="C297" s="10"/>
+      <c r="D297" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="F297" s="1"/>
-      <c r="G297" s="1"/>
+      <c r="E297" s="10"/>
+      <c r="F297" s="10"/>
+      <c r="G297" s="10"/>
       <c r="H297" s="1"/>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="8" t="s">
         <v>621</v>
       </c>
@@ -63055,42 +63076,51 @@
       <c r="G298" s="8"/>
       <c r="H298" s="1"/>
     </row>
-    <row r="299" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A299" s="1" t="s">
+    <row r="299" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A299" s="7" t="s">
         <v>623</v>
       </c>
-      <c r="D299" s="1" t="s">
+      <c r="B299" s="7"/>
+      <c r="C299" s="7"/>
+      <c r="D299" s="7" t="s">
         <v>624</v>
       </c>
-      <c r="F299" s="1"/>
-      <c r="G299" s="1"/>
+      <c r="E299" s="7"/>
+      <c r="F299" s="7"/>
+      <c r="G299" s="7"/>
       <c r="H299" s="1" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="300" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A300" s="1" t="s">
+    <row r="300" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A300" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="D300" s="1" t="s">
+      <c r="B300" s="7"/>
+      <c r="C300" s="7"/>
+      <c r="D300" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="F300" s="1"/>
-      <c r="G300" s="1"/>
+      <c r="E300" s="7"/>
+      <c r="F300" s="7"/>
+      <c r="G300" s="7"/>
       <c r="H300" s="1"/>
     </row>
-    <row r="301" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A301" s="1" t="s">
+    <row r="301" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A301" s="6" t="s">
         <v>626</v>
       </c>
-      <c r="D301" s="1" t="s">
+      <c r="B301" s="6"/>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="F301" s="1"/>
-      <c r="G301" s="1"/>
+      <c r="E301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="6"/>
       <c r="H301" s="1"/>
     </row>
-    <row r="302" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>628</v>
       </c>
@@ -63101,7 +63131,7 @@
       <c r="G302" s="1"/>
       <c r="H302" s="1"/>
     </row>
-    <row r="303" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>630</v>
       </c>
@@ -63112,7 +63142,7 @@
       <c r="G303" s="1"/>
       <c r="H303" s="1"/>
     </row>
-    <row r="304" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A304" s="7" t="s">
         <v>632</v>
       </c>
@@ -63126,7 +63156,7 @@
       <c r="G304" s="7"/>
       <c r="H304" s="1"/>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="7" t="s">
         <v>636</v>
       </c>
@@ -63140,7 +63170,7 @@
       <c r="G305" s="7"/>
       <c r="H305" s="1"/>
     </row>
-    <row r="306" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A306" s="7" t="s">
         <v>634</v>
       </c>
@@ -63154,7 +63184,7 @@
       <c r="G306" s="7"/>
       <c r="H306" s="1"/>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="7" t="s">
         <v>638</v>
       </c>

</xml_diff>